<commit_message>
Downgrade Python version to 3.11
</commit_message>
<xml_diff>
--- a/output/WhatsApp Image 2025-03-01 at 12.42.16_9bfb0832.xlsx
+++ b/output/WhatsApp Image 2025-03-01 at 12.42.16_9bfb0832.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,36 +436,6 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Filename</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Format</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Mode</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Width</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Height</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>Extracted Text</t>
         </is>
       </c>
@@ -473,36 +443,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>WhatsApp Image 2025-03-01 at 12.42.16_9bfb0832.jpg</t>
+          <t>ss 220854 30 pom poe vawn/xoanten</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
-          <t>JPEG</t>
+          <t>oo? «SY8stUzESBOSE “took xan REA Or swntO ant Soepore SEE T=! ta feud 4a od o00t</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
-          <t>RGB</t>
+          <t>ETAT &gt;055 30 tng T/G0S 295 tdang S05 ag</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
-          <t>1280x960</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1280</v>
-      </c>
-      <c r="F2" t="n">
-        <v>960</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ss 220854 30 pom poe vawn/xoanten
-oo? «SY8stUzESBOSE “took xan REA Or swntO ant Soepore SEE T=! ta feud 4a od o00t
-ETAT &gt;055 30 tng T/G0S 295 tdang S05 ag
-Teter Sc/e0/o aa</t>
+          <t>Teter Sc/e0/o aa</t>
         </is>
       </c>
     </row>

</xml_diff>